<commit_message>
deleted test script from expert folder
</commit_message>
<xml_diff>
--- a/TEST/Setup.xlsx
+++ b/TEST/Setup.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6FA5B565-3C34-47B4-8D96-D4561DE56052}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8BF35792-50BC-416F-8D10-FF780725AB51}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="32">
   <si>
     <t>Pair</t>
   </si>
@@ -50,6 +50,72 @@
   </si>
   <si>
     <t>EURUSD</t>
+  </si>
+  <si>
+    <t>EURGBP</t>
+  </si>
+  <si>
+    <t>EURAUD</t>
+  </si>
+  <si>
+    <t>EURCHF</t>
+  </si>
+  <si>
+    <t>EURJPY</t>
+  </si>
+  <si>
+    <t>GBPCHF</t>
+  </si>
+  <si>
+    <t>CADJPY</t>
+  </si>
+  <si>
+    <t>GBPJPY</t>
+  </si>
+  <si>
+    <t>AUDNZD</t>
+  </si>
+  <si>
+    <t>AUDCAD</t>
+  </si>
+  <si>
+    <t>AUDCHF</t>
+  </si>
+  <si>
+    <t>AUDJPY</t>
+  </si>
+  <si>
+    <t>CHFJPY</t>
+  </si>
+  <si>
+    <t>EURNZD</t>
+  </si>
+  <si>
+    <t>EURCAD</t>
+  </si>
+  <si>
+    <t>CADCHF</t>
+  </si>
+  <si>
+    <t>NZDJPY</t>
+  </si>
+  <si>
+    <t>NZDUSD</t>
+  </si>
+  <si>
+    <t>GBPAUD</t>
+  </si>
+  <si>
+    <t>NZDCHF</t>
+  </si>
+  <si>
+    <t>GBPCAD</t>
+  </si>
+  <si>
+    <t>GBPNZD</t>
+  </si>
+  <si>
+    <t>NZDCAD</t>
   </si>
 </sst>
 </file>
@@ -367,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,7 +460,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>8137401</v>
+        <v>8137101</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -405,7 +471,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>8137402</v>
+        <v>8137102</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -416,7 +482,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>8137403</v>
+        <v>8137103</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -427,7 +493,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>8137404</v>
+        <v>8137104</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -438,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>8137405</v>
+        <v>8137105</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -449,7 +515,557 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>8137406</v>
+        <v>8137106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>8137107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>8137108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>8137109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>8137110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>8137111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>8137112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>8137113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>8137114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>8137115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>8137116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>8137117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>8137118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>8137119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>8137120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>8137121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>8137122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>8137123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>8137124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>8137125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>8137126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>8137127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>8137128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>8137301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>8137302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>8137303</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>8137304</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>8137305</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>8137306</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>8137307</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>8137308</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>8137309</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>8137310</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>8137311</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>8137312</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>8137313</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>8137314</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>8137315</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>8137316</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>8137317</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>8137318</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>8137319</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>8137320</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>8137321</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>8137322</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>8137323</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>8137324</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>8137325</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55">
+        <v>8137326</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56">
+        <v>8137327</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57">
+        <v>8137328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>